<commit_message>
change the tcfd rules to better representation
</commit_message>
<xml_diff>
--- a/data/tcfd接露指引.xlsx
+++ b/data/tcfd接露指引.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattis\Desktop\VSCode\rag_test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattis\Desktop\VSCode\rag_for_tcfd_reports\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F952A3-EBD6-4840-A39E-777D2D522A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BF8B8C-B9A8-4812-A174-DB1AF95B198A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{A01FB36B-7D90-4A56-93BF-375EDAB9840C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A01FB36B-7D90-4A56-93BF-375EDAB9840C}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -793,17 +793,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA9E989E-C8C2-47E4-80EE-129D0D454BCA}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:B3742"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="121.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.625" customWidth="1"/>
+    <col min="2" max="2" width="121.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -811,7 +811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -819,7 +819,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -827,7 +827,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>95</v>
       </c>
@@ -835,7 +835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -843,7 +843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -851,7 +851,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -859,7 +859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -867,7 +867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -875,7 +875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -883,7 +883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -891,7 +891,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -899,7 +899,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -907,7 +907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -915,7 +915,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -923,7 +923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -931,7 +931,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -939,7 +939,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -947,7 +947,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -955,7 +955,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -963,7 +963,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -971,7 +971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -979,7 +979,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -987,7 +987,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -995,7 +995,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>

</xml_diff>